<commit_message>
Vinh quang - Danh dự - Trách nhiệm
Hoàng plan 20191112
</commit_message>
<xml_diff>
--- a/_wallpage/HoangPlan.xlsx
+++ b/_wallpage/HoangPlan.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
     <sheet name="Plan" sheetId="2" r:id="rId2"/>
     <sheet name="CheckList_Web_20190713" sheetId="3" r:id="rId3"/>
     <sheet name="Timetable" sheetId="4" r:id="rId4"/>
+    <sheet name="RESTfull" sheetId="5" r:id="rId5"/>
+    <sheet name="Draft" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
   <si>
     <t>Time</t>
   </si>
@@ -343,6 +345,87 @@
   </si>
   <si>
     <t>Family</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>RESTfull</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>PCX 150</t>
+  </si>
+  <si>
+    <t>Xpander AT 720</t>
+  </si>
+  <si>
+    <t>ENG -960</t>
+  </si>
+  <si>
+    <t>FRN - B</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>Malta - 23000</t>
+  </si>
+  <si>
+    <t>Elec -10</t>
+  </si>
+  <si>
+    <t>E-bik 7.5</t>
+  </si>
+  <si>
+    <t>Pas 2.5 x 2</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Gap2</t>
+  </si>
+  <si>
+    <t>Gap1</t>
+  </si>
+  <si>
+    <t>Văn bằng 2 tiếng Anh</t>
+  </si>
+  <si>
+    <t>Công ty nước ngoài lương 10.000 USD/tháng</t>
+  </si>
+  <si>
+    <t>Lập công ty riêng</t>
+  </si>
+  <si>
+    <t>Cửa hàng bán đồ trẻ em</t>
+  </si>
+  <si>
+    <t>Nhà 15 tỉ</t>
+  </si>
+  <si>
+    <t>Xe 7 chỗ máy dầu</t>
+  </si>
+  <si>
+    <t>Lấy bằng Thạc sĩ</t>
+  </si>
+  <si>
+    <t>Lấy bằng tiến sĩ kinh tế</t>
+  </si>
+  <si>
+    <t>Định cư nước ngoài theo diện doanh nhân</t>
+  </si>
+  <si>
+    <t>Cống hiến</t>
   </si>
 </sst>
 </file>
@@ -352,7 +435,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,12 +453,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,12 +482,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,6 +596,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -525,7 +618,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,6 +1191,12 @@
                 <c:pt idx="4">
                   <c:v>700</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1123,11 +1221,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="260075000"/>
-        <c:axId val="260075392"/>
+        <c:axId val="413672880"/>
+        <c:axId val="413670528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="260075000"/>
+        <c:axId val="413672880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1239,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260075392"/>
+        <c:crossAx val="413670528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1149,7 +1247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260075392"/>
+        <c:axId val="413670528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1164,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260075000"/>
+        <c:crossAx val="413672880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1275,12 +1373,12 @@
         <c:gapWidth val="100"/>
         <c:gapDepth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="260072648"/>
-        <c:axId val="260073040"/>
+        <c:axId val="413671704"/>
+        <c:axId val="413668176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="260072648"/>
+        <c:axId val="413671704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1391,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260073040"/>
+        <c:crossAx val="413668176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1301,7 +1399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260073040"/>
+        <c:axId val="413668176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1319,7 +1417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260072648"/>
+        <c:crossAx val="413671704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1345,16 +1443,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133348</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:rowOff>40663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
+      <xdr:colOff>189033</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>188302</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1698,15 +1796,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM8"/>
+  <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -2276,155 +2375,317 @@
       <c r="F7">
         <v>700</v>
       </c>
+      <c r="G7">
+        <v>700</v>
+      </c>
+      <c r="H7">
+        <v>700</v>
+      </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <f>B7-B4</f>
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="19">
+        <f>IF(ISNUMBER($B$7),B7-B4,"")</f>
         <v>0</v>
       </c>
-      <c r="C8" s="22">
-        <f t="shared" ref="C8:AL8" si="2">C7-C4</f>
+      <c r="C8" s="19">
+        <f t="shared" ref="C8:F8" si="2">IF(ISNUMBER(C7),C7-C4,"")</f>
         <v>-10</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="19">
         <f t="shared" si="2"/>
         <v>-20</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="19">
         <f t="shared" si="2"/>
         <v>-38.5</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="19">
         <f t="shared" si="2"/>
         <v>-57</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>-775.5</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>-794</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>-812.5</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>-831</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="2"/>
-        <v>-849.5</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>-868</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="2"/>
-        <v>-886.5</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="2"/>
-        <v>-905</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="2"/>
-        <v>-923.5</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="2"/>
-        <v>-942</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="2"/>
-        <v>-968.5</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="2"/>
-        <v>-995</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="2"/>
-        <v>-1021.5</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="2"/>
-        <v>-1048</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="2"/>
-        <v>-1074.5</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="2"/>
-        <v>-1101</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="2"/>
-        <v>-1127.5</v>
-      </c>
-      <c r="X8">
-        <f t="shared" si="2"/>
-        <v>-1154</v>
-      </c>
-      <c r="Y8">
-        <f t="shared" si="2"/>
-        <v>-1180.5</v>
-      </c>
-      <c r="Z8">
-        <f t="shared" si="2"/>
-        <v>-1207</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="2"/>
-        <v>-1233.5</v>
-      </c>
-      <c r="AB8">
-        <f t="shared" si="2"/>
-        <v>-1260</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="2"/>
-        <v>-1298.5</v>
-      </c>
-      <c r="AD8">
-        <f t="shared" si="2"/>
-        <v>-1337</v>
-      </c>
-      <c r="AE8">
-        <f t="shared" si="2"/>
-        <v>-1375.5</v>
-      </c>
-      <c r="AF8">
-        <f t="shared" si="2"/>
-        <v>-1414</v>
-      </c>
-      <c r="AG8">
-        <f t="shared" si="2"/>
-        <v>-1452.5</v>
-      </c>
-      <c r="AH8">
-        <f t="shared" si="2"/>
-        <v>-1491</v>
-      </c>
-      <c r="AI8">
-        <f t="shared" si="2"/>
-        <v>-1529.5</v>
-      </c>
-      <c r="AJ8">
-        <f t="shared" si="2"/>
-        <v>-1568</v>
-      </c>
-      <c r="AK8">
-        <f t="shared" si="2"/>
-        <v>-1606.5</v>
-      </c>
-      <c r="AL8">
-        <f t="shared" si="2"/>
-        <v>-1645</v>
+      <c r="G8" s="19">
+        <f t="shared" ref="G8" si="3">IF(ISNUMBER(G7),G7-G4,"")</f>
+        <v>-75.5</v>
+      </c>
+      <c r="H8" s="19">
+        <f t="shared" ref="H8" si="4">IF(ISNUMBER(H7),H7-H4,"")</f>
+        <v>-94</v>
+      </c>
+      <c r="I8" s="19" t="str">
+        <f t="shared" ref="I8" si="5">IF(ISNUMBER(I7),I7-I4,"")</f>
+        <v/>
+      </c>
+      <c r="J8" s="19" t="str">
+        <f t="shared" ref="J8" si="6">IF(ISNUMBER(J7),J7-J4,"")</f>
+        <v/>
+      </c>
+      <c r="K8" s="19" t="str">
+        <f t="shared" ref="K8" si="7">IF(ISNUMBER(K7),K7-K4,"")</f>
+        <v/>
+      </c>
+      <c r="L8" s="19" t="str">
+        <f t="shared" ref="L8" si="8">IF(ISNUMBER(L7),L7-L4,"")</f>
+        <v/>
+      </c>
+      <c r="M8" s="19" t="str">
+        <f t="shared" ref="M8" si="9">IF(ISNUMBER(M7),M7-M4,"")</f>
+        <v/>
+      </c>
+      <c r="N8" s="19" t="str">
+        <f t="shared" ref="N8" si="10">IF(ISNUMBER(N7),N7-N4,"")</f>
+        <v/>
+      </c>
+      <c r="O8" s="19" t="str">
+        <f t="shared" ref="O8" si="11">IF(ISNUMBER(O7),O7-O4,"")</f>
+        <v/>
+      </c>
+      <c r="P8" s="19" t="str">
+        <f t="shared" ref="P8" si="12">IF(ISNUMBER(P7),P7-P4,"")</f>
+        <v/>
+      </c>
+      <c r="Q8" s="19" t="str">
+        <f t="shared" ref="Q8" si="13">IF(ISNUMBER(Q7),Q7-Q4,"")</f>
+        <v/>
+      </c>
+      <c r="R8" s="19" t="str">
+        <f t="shared" ref="R8" si="14">IF(ISNUMBER(R7),R7-R4,"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="19" t="str">
+        <f t="shared" ref="S8" si="15">IF(ISNUMBER(S7),S7-S4,"")</f>
+        <v/>
+      </c>
+      <c r="T8" s="19" t="str">
+        <f t="shared" ref="T8" si="16">IF(ISNUMBER(T7),T7-T4,"")</f>
+        <v/>
+      </c>
+      <c r="U8" s="19" t="str">
+        <f t="shared" ref="U8" si="17">IF(ISNUMBER(U7),U7-U4,"")</f>
+        <v/>
+      </c>
+      <c r="V8" s="19" t="str">
+        <f t="shared" ref="V8" si="18">IF(ISNUMBER(V7),V7-V4,"")</f>
+        <v/>
+      </c>
+      <c r="W8" s="19" t="str">
+        <f t="shared" ref="W8" si="19">IF(ISNUMBER(W7),W7-W4,"")</f>
+        <v/>
+      </c>
+      <c r="X8" s="19" t="str">
+        <f t="shared" ref="X8" si="20">IF(ISNUMBER(X7),X7-X4,"")</f>
+        <v/>
+      </c>
+      <c r="Y8" s="19" t="str">
+        <f t="shared" ref="Y8" si="21">IF(ISNUMBER(Y7),Y7-Y4,"")</f>
+        <v/>
+      </c>
+      <c r="Z8" s="19" t="str">
+        <f t="shared" ref="Z8" si="22">IF(ISNUMBER(Z7),Z7-Z4,"")</f>
+        <v/>
+      </c>
+      <c r="AA8" s="19" t="str">
+        <f t="shared" ref="AA8" si="23">IF(ISNUMBER(AA7),AA7-AA4,"")</f>
+        <v/>
+      </c>
+      <c r="AB8" s="19" t="str">
+        <f t="shared" ref="AB8" si="24">IF(ISNUMBER(AB7),AB7-AB4,"")</f>
+        <v/>
+      </c>
+      <c r="AC8" s="19" t="str">
+        <f t="shared" ref="AC8" si="25">IF(ISNUMBER(AC7),AC7-AC4,"")</f>
+        <v/>
+      </c>
+      <c r="AD8" s="19" t="str">
+        <f t="shared" ref="AD8" si="26">IF(ISNUMBER(AD7),AD7-AD4,"")</f>
+        <v/>
+      </c>
+      <c r="AE8" s="19" t="str">
+        <f t="shared" ref="AE8" si="27">IF(ISNUMBER(AE7),AE7-AE4,"")</f>
+        <v/>
+      </c>
+      <c r="AF8" s="19" t="str">
+        <f t="shared" ref="AF8" si="28">IF(ISNUMBER(AF7),AF7-AF4,"")</f>
+        <v/>
+      </c>
+      <c r="AG8" s="19" t="str">
+        <f t="shared" ref="AG8" si="29">IF(ISNUMBER(AG7),AG7-AG4,"")</f>
+        <v/>
+      </c>
+      <c r="AH8" s="19" t="str">
+        <f t="shared" ref="AH8" si="30">IF(ISNUMBER(AH7),AH7-AH4,"")</f>
+        <v/>
+      </c>
+      <c r="AI8" s="19" t="str">
+        <f t="shared" ref="AI8" si="31">IF(ISNUMBER(AI7),AI7-AI4,"")</f>
+        <v/>
+      </c>
+      <c r="AJ8" s="19" t="str">
+        <f t="shared" ref="AJ8" si="32">IF(ISNUMBER(AJ7),AJ7-AJ4,"")</f>
+        <v/>
+      </c>
+      <c r="AK8" s="19" t="str">
+        <f t="shared" ref="AK8" si="33">IF(ISNUMBER(AK7),AK7-AK4,"")</f>
+        <v/>
+      </c>
+      <c r="AL8" s="19" t="str">
+        <f t="shared" ref="AL8" si="34">IF(ISNUMBER(AL7),AL7-AL4,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="20">
+        <f>IF(ISNUMBER(B7),B7-B6,"")</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="20">
+        <f t="shared" ref="C9:AL9" si="35">IF(ISNUMBER(C7),C7-C6,"")</f>
+        <v>-63.888888888888914</v>
+      </c>
+      <c r="D9" s="20">
+        <f t="shared" si="35"/>
+        <v>-127.77777777777783</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="35"/>
+        <v>-191.66666666666674</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="35"/>
+        <v>-255.55555555555566</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="35"/>
+        <v>-319.44444444444457</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="35"/>
+        <v>-383.33333333333348</v>
+      </c>
+      <c r="I9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="J9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="K9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="L9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="M9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="N9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="O9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="P9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="Q9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="R9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="S9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="T9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="U9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="V9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="W9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="X9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="Y9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="Z9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AA9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AB9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AC9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AE9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AF9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AG9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AH9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AI9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AJ9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AK9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AL9" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -2439,7 +2700,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -3121,7 +3382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -3139,17 +3400,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
@@ -3184,13 +3445,13 @@
       <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="13" t="s">
         <v>82</v>
       </c>
@@ -3202,13 +3463,13 @@
       <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="13" t="s">
         <v>101</v>
       </c>
@@ -3223,13 +3484,13 @@
       <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="13" t="s">
         <v>100</v>
       </c>
@@ -3244,13 +3505,13 @@
       <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="13" t="s">
         <v>97</v>
       </c>
@@ -3265,13 +3526,13 @@
       <c r="B8" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="16" t="s">
         <v>98</v>
       </c>
@@ -3286,13 +3547,13 @@
       <c r="B9" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="16" t="s">
         <v>99</v>
       </c>
@@ -3307,13 +3568,13 @@
       <c r="B10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="16" t="s">
         <v>86</v>
       </c>
@@ -3365,4 +3626,381 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="18"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="18"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hoang plan Update timetable
</commit_message>
<xml_diff>
--- a/_wallpage/HoangPlan.xlsx
+++ b/_wallpage/HoangPlan.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Property" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan" sheetId="2" r:id="rId2"/>
-    <sheet name="CheckList_Web_20190713" sheetId="3" r:id="rId3"/>
-    <sheet name="Timetable" sheetId="4" r:id="rId4"/>
-    <sheet name="RESTfull" sheetId="5" r:id="rId5"/>
-    <sheet name="Draft" sheetId="6" r:id="rId6"/>
+    <sheet name="Timetable (2)" sheetId="7" r:id="rId1"/>
+    <sheet name="Property" sheetId="1" r:id="rId2"/>
+    <sheet name="Plan" sheetId="2" r:id="rId3"/>
+    <sheet name="CheckList_Web_20190713" sheetId="3" r:id="rId4"/>
+    <sheet name="Timetable" sheetId="4" r:id="rId5"/>
+    <sheet name="RESTfull" sheetId="5" r:id="rId6"/>
+    <sheet name="Draft" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="143">
   <si>
     <t>Time</t>
   </si>
@@ -380,15 +381,6 @@
     <t>Malta - 23000</t>
   </si>
   <si>
-    <t>Elec -10</t>
-  </si>
-  <si>
-    <t>E-bik 7.5</t>
-  </si>
-  <si>
-    <t>Pas 2.5 x 2</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -429,6 +421,39 @@
   </si>
   <si>
     <t>Tập cách đặt câu hỏi và trả lời</t>
+  </si>
+  <si>
+    <t>Xe đạp điện 7.5</t>
+  </si>
+  <si>
+    <t>Lò vi sóng có nướng  2.5 x2</t>
+  </si>
+  <si>
+    <t>Máy giặt electronic 10.</t>
+  </si>
+  <si>
+    <t>Get up</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Physical excersise</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Breaking time</t>
+  </si>
+  <si>
+    <t>Housework</t>
+  </si>
+  <si>
+    <t>Go to Church</t>
+  </si>
+  <si>
+    <t>IT</t>
   </si>
 </sst>
 </file>
@@ -489,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -558,11 +583,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -621,6 +672,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,11 +1296,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="217320400"/>
-        <c:axId val="217320792"/>
+        <c:axId val="252648976"/>
+        <c:axId val="252651720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="217320400"/>
+        <c:axId val="252648976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1241,7 +1313,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217320792"/>
+        <c:crossAx val="252651720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1249,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217320792"/>
+        <c:axId val="252651720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1335,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217320400"/>
+        <c:crossAx val="252648976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1373,24 +1445,25 @@
         <c:gapWidth val="100"/>
         <c:gapDepth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="217321184"/>
-        <c:axId val="217318832"/>
+        <c:axId val="252654464"/>
+        <c:axId val="252654856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="217321184"/>
+        <c:axId val="252654464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217318832"/>
+        <c:crossAx val="252654856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1398,7 +1471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217318832"/>
+        <c:axId val="252654856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1409,19 +1482,21 @@
         <c:majorGridlines/>
         <c:minorGridlines/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217321184"/>
+        <c:crossAx val="252654464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1793,6 +1868,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="9" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="26">
+        <v>5</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="26">
+        <v>6.3</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
+        <v>8</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
+      <c r="C9" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26">
+        <v>10</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="2:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="26">
+        <v>12</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
+        <v>13</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I15" s="31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26">
+        <v>15</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="2:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26">
+        <v>17</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="2:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="26">
+        <v>19</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="2:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
+      <c r="C21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="26">
+        <v>21</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="2:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
+      <c r="C23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="26">
+        <v>23</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="26"/>
+      <c r="C25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="82">
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM9"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -2381,7 +3010,7 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" s="19">
         <f>IF(ISNUMBER($B$7),B7-B4,"")</f>
@@ -2534,7 +3163,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B9" s="20">
         <f>IF(ISNUMBER(B7),B7-B6,"")</f>
@@ -2692,7 +3321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -3010,7 +3639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
@@ -3375,12 +4004,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +4254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
@@ -3679,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -3816,12 +4445,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,7 +4527,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3906,7 +4535,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3914,7 +4543,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3922,7 +4551,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3930,7 +4559,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3938,7 +4567,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3946,7 +4575,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3954,7 +4583,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3962,7 +4591,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3970,7 +4599,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3978,7 +4607,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3986,7 +4615,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3994,7 +4623,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4002,7 +4631,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>